<commit_message>
push code sua mau
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/HoaDonDienTu/BANG_KE_CHI_TIET_HOA_DON_DIEN_TU.xlsx
+++ b/API/wwwroot/docs/HoaDonDienTu/BANG_KE_CHI_TIET_HOA_DON_DIEN_TU.xlsx
@@ -14,7 +14,8 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>BẢNG KÊ CHI TIẾT HÓA ĐƠN ĐIỆN TỬ</t>
   </si>
@@ -165,6 +166,12 @@
   </si>
   <si>
     <t>Người lập</t>
+  </si>
+  <si>
+    <t>Tỷ lệ tính thuế GTGT</t>
+  </si>
+  <si>
+    <t>Thuế GTGT được giảm</t>
   </si>
 </sst>
 </file>
@@ -285,12 +292,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
@@ -298,6 +299,12 @@
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS5"/>
+  <dimension ref="A1:AU5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AN21" sqref="AN21"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,127 +651,131 @@
     <col min="23" max="23" width="23.5546875" customWidth="1"/>
     <col min="24" max="24" width="19.109375" customWidth="1"/>
     <col min="25" max="25" width="22" customWidth="1"/>
-    <col min="26" max="26" width="22.88671875" customWidth="1"/>
-    <col min="27" max="27" width="24.77734375" customWidth="1"/>
-    <col min="28" max="28" width="25.88671875" customWidth="1"/>
-    <col min="29" max="29" width="18.44140625" customWidth="1"/>
-    <col min="30" max="30" width="17.21875" customWidth="1"/>
-    <col min="31" max="31" width="15.109375" customWidth="1"/>
-    <col min="32" max="32" width="16.5546875" customWidth="1"/>
-    <col min="33" max="33" width="12.33203125" customWidth="1"/>
-    <col min="34" max="34" width="13" customWidth="1"/>
-    <col min="35" max="35" width="15" customWidth="1"/>
-    <col min="36" max="36" width="30.21875" customWidth="1"/>
-    <col min="37" max="37" width="15.33203125" customWidth="1"/>
-    <col min="38" max="38" width="23.6640625" customWidth="1"/>
-    <col min="39" max="39" width="18.77734375" customWidth="1"/>
-    <col min="40" max="40" width="21.21875" customWidth="1"/>
-    <col min="41" max="41" width="22.109375" customWidth="1"/>
-    <col min="42" max="42" width="25.6640625" customWidth="1"/>
-    <col min="43" max="43" width="31.44140625" customWidth="1"/>
-    <col min="44" max="44" width="16.109375" customWidth="1"/>
-    <col min="45" max="45" width="27.33203125" customWidth="1"/>
+    <col min="26" max="28" width="22.88671875" customWidth="1"/>
+    <col min="29" max="29" width="24.77734375" customWidth="1"/>
+    <col min="30" max="30" width="25.88671875" customWidth="1"/>
+    <col min="31" max="31" width="18.44140625" customWidth="1"/>
+    <col min="32" max="32" width="17.21875" customWidth="1"/>
+    <col min="33" max="33" width="15.109375" customWidth="1"/>
+    <col min="34" max="34" width="16.5546875" customWidth="1"/>
+    <col min="35" max="35" width="12.33203125" customWidth="1"/>
+    <col min="36" max="36" width="13" customWidth="1"/>
+    <col min="37" max="37" width="15" customWidth="1"/>
+    <col min="38" max="38" width="30.21875" customWidth="1"/>
+    <col min="39" max="39" width="15.33203125" customWidth="1"/>
+    <col min="40" max="40" width="23.6640625" customWidth="1"/>
+    <col min="41" max="41" width="18.77734375" customWidth="1"/>
+    <col min="42" max="42" width="21.21875" customWidth="1"/>
+    <col min="43" max="43" width="22.109375" customWidth="1"/>
+    <col min="44" max="44" width="25.6640625" customWidth="1"/>
+    <col min="45" max="45" width="31.44140625" customWidth="1"/>
+    <col min="46" max="46" width="16.109375" customWidth="1"/>
+    <col min="47" max="47" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:47" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5"/>
-      <c r="AM1" s="5"/>
-      <c r="AN1" s="5"/>
-      <c r="AO1" s="5"/>
-      <c r="AP1" s="5"/>
-      <c r="AQ1" s="5"/>
-      <c r="AR1" s="5"/>
-      <c r="AS1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="8"/>
+      <c r="AP1" s="8"/>
+      <c r="AQ1" s="8"/>
+      <c r="AR1" s="8"/>
+      <c r="AS1" s="8"/>
+      <c r="AT1" s="8"/>
+      <c r="AU1" s="8"/>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6"/>
-      <c r="AH2" s="6"/>
-      <c r="AI2" s="6"/>
-      <c r="AJ2" s="6"/>
-      <c r="AK2" s="6"/>
-      <c r="AL2" s="6"/>
-      <c r="AM2" s="6"/>
-      <c r="AN2" s="6"/>
-      <c r="AO2" s="6"/>
-      <c r="AP2" s="6"/>
-      <c r="AQ2" s="6"/>
-      <c r="AR2" s="6"/>
-      <c r="AS2" s="6"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="9"/>
+      <c r="AO2" s="9"/>
+      <c r="AP2" s="9"/>
+      <c r="AQ2" s="9"/>
+      <c r="AR2" s="9"/>
+      <c r="AS2" s="9"/>
+      <c r="AT2" s="9"/>
+      <c r="AU2" s="9"/>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -772,7 +783,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -852,114 +863,122 @@
         <v>27</v>
       </c>
       <c r="AA4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AB4" s="4" t="s">
+      <c r="AD4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AC4" s="4" t="s">
+      <c r="AE4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AD4" s="4" t="s">
+      <c r="AF4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AE4" s="4" t="s">
+      <c r="AG4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AF4" s="4" t="s">
+      <c r="AH4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AG4" s="4" t="s">
+      <c r="AI4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AH4" s="4" t="s">
+      <c r="AJ4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AI4" s="4" t="s">
+      <c r="AK4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AJ4" s="4" t="s">
+      <c r="AL4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AK4" s="4" t="s">
+      <c r="AM4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AL4" s="4" t="s">
+      <c r="AN4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AM4" s="4" t="s">
+      <c r="AO4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AN4" s="4" t="s">
+      <c r="AP4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AO4" s="4" t="s">
+      <c r="AQ4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AP4" s="4" t="s">
+      <c r="AR4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AQ4" s="4" t="s">
+      <c r="AS4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AR4" s="4" t="s">
+      <c r="AT4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AS4" s="4" t="s">
+      <c r="AU4" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:45" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="7"/>
-      <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
-      <c r="AG5" s="7"/>
-      <c r="AH5" s="7"/>
-      <c r="AI5" s="7"/>
-      <c r="AJ5" s="7"/>
-      <c r="AK5" s="7"/>
-      <c r="AL5" s="7"/>
-      <c r="AM5" s="7"/>
-      <c r="AN5" s="7"/>
-      <c r="AO5" s="7"/>
-      <c r="AP5" s="7"/>
-      <c r="AQ5" s="7"/>
-      <c r="AR5" s="7"/>
-      <c r="AS5" s="7"/>
+    <row r="5" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="5"/>
+      <c r="AQ5" s="5"/>
+      <c r="AR5" s="5"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="5"/>
+      <c r="AU5" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:AS1"/>
-    <mergeCell ref="A2:AS2"/>
+    <mergeCell ref="A1:AU1"/>
+    <mergeCell ref="A2:AU2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
push code sua file bang ke chi tiet excel
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/HoaDonDienTu/BANG_KE_CHI_TIET_HOA_DON_DIEN_TU.xlsx
+++ b/API/wwwroot/docs/HoaDonDienTu/BANG_KE_CHI_TIET_HOA_DON_DIEN_TU.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>BẢNG KÊ CHI TIẾT HÓA ĐƠN ĐIỆN TỬ</t>
   </si>
@@ -117,9 +116,6 @@
     <t>Tổng tiền thanh toán quy đổi</t>
   </si>
   <si>
-    <t>Hàng khuyến mại</t>
-  </si>
-  <si>
     <t>Mã quy cách</t>
   </si>
   <si>
@@ -172,6 +168,12 @@
   </si>
   <si>
     <t>Thuế GTGT được giảm</t>
+  </si>
+  <si>
+    <t>Tính chất hàng hóa</t>
+  </si>
+  <si>
+    <t>Thông tin hóa đơn liên quan</t>
   </si>
 </sst>
 </file>
@@ -619,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU5"/>
+  <dimension ref="A1:AV5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AT17" sqref="AT17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,11 +671,12 @@
     <col min="43" max="43" width="22.109375" customWidth="1"/>
     <col min="44" max="44" width="25.6640625" customWidth="1"/>
     <col min="45" max="45" width="31.44140625" customWidth="1"/>
-    <col min="46" max="46" width="16.109375" customWidth="1"/>
-    <col min="47" max="47" width="27.33203125" customWidth="1"/>
+    <col min="46" max="46" width="39.109375" customWidth="1"/>
+    <col min="47" max="47" width="16.109375" customWidth="1"/>
+    <col min="48" max="48" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:48" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -723,8 +726,9 @@
       <c r="AS1" s="8"/>
       <c r="AT1" s="8"/>
       <c r="AU1" s="8"/>
+      <c r="AV1" s="8"/>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -774,8 +778,9 @@
       <c r="AS2" s="9"/>
       <c r="AT2" s="9"/>
       <c r="AU2" s="9"/>
+      <c r="AV2" s="9"/>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -783,7 +788,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -863,10 +868,10 @@
         <v>27</v>
       </c>
       <c r="AA4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB4" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="AC4" s="4" t="s">
         <v>28</v>
@@ -875,58 +880,61 @@
         <v>29</v>
       </c>
       <c r="AE4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AF4" s="4" t="s">
+      <c r="AG4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AG4" s="4" t="s">
+      <c r="AH4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH4" s="4" t="s">
+      <c r="AI4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI4" s="4" t="s">
+      <c r="AJ4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ4" s="4" t="s">
+      <c r="AK4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AK4" s="4" t="s">
+      <c r="AL4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AL4" s="4" t="s">
+      <c r="AM4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AM4" s="4" t="s">
+      <c r="AN4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AN4" s="4" t="s">
+      <c r="AO4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AO4" s="4" t="s">
+      <c r="AP4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AP4" s="4" t="s">
+      <c r="AQ4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AQ4" s="4" t="s">
+      <c r="AR4" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AR4" s="4" t="s">
+      <c r="AS4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AS4" s="4" t="s">
+      <c r="AT4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AU4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AT4" s="4" t="s">
+      <c r="AV4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AU4" s="4" t="s">
-        <v>46</v>
-      </c>
     </row>
-    <row r="5" spans="1:47" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
@@ -974,11 +982,12 @@
       <c r="AS5" s="5"/>
       <c r="AT5" s="5"/>
       <c r="AU5" s="5"/>
+      <c r="AV5" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:AU1"/>
-    <mergeCell ref="A2:AU2"/>
+    <mergeCell ref="A1:AV1"/>
+    <mergeCell ref="A2:AV2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Bug #1846: 0.9.Khac phuc HDBK T06.2022 - LK 2022-06-24
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/HoaDonDienTu/BANG_KE_CHI_TIET_HOA_DON_DIEN_TU.xlsx
+++ b/API/wwwroot/docs/HoaDonDienTu/BANG_KE_CHI_TIET_HOA_DON_DIEN_TU.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT\bill-back-end\API\wwwroot\docs\HoaDonDienTu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bill-back-end\API\wwwroot\docs\HoaDonDienTu\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A91715-437E-41CA-9982-DC7004C153F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20376" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -179,12 +188,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -215,15 +224,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Times New Roman"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <charset val="163"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -235,7 +251,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -246,21 +262,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right style="thin">
-        <color theme="6"/>
-      </right>
-      <top style="thin">
-        <color theme="6"/>
-      </top>
-      <bottom style="thin">
-        <color theme="6"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -278,11 +279,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="hair">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -291,25 +308,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{1BAE8359-BB78-40ED-8F2F-283B0F1F8CA0}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -620,167 +635,167 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.875" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="30" customWidth="1"/>
-    <col min="8" max="8" width="36.5546875" customWidth="1"/>
-    <col min="9" max="9" width="19.21875" customWidth="1"/>
-    <col min="10" max="10" width="31.88671875" customWidth="1"/>
+    <col min="8" max="8" width="36.5" customWidth="1"/>
+    <col min="9" max="9" width="19.25" customWidth="1"/>
+    <col min="10" max="10" width="31.875" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" customWidth="1"/>
-    <col min="13" max="13" width="13.21875" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" customWidth="1"/>
-    <col min="15" max="15" width="30.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10.5" customWidth="1"/>
+    <col min="13" max="13" width="13.25" customWidth="1"/>
+    <col min="14" max="14" width="13.625" customWidth="1"/>
+    <col min="15" max="15" width="30.5" customWidth="1"/>
     <col min="16" max="16" width="21" customWidth="1"/>
-    <col min="17" max="17" width="9.21875" customWidth="1"/>
-    <col min="18" max="18" width="14.44140625" customWidth="1"/>
-    <col min="19" max="19" width="17.21875" customWidth="1"/>
-    <col min="20" max="20" width="19.6640625" customWidth="1"/>
-    <col min="21" max="21" width="22.88671875" customWidth="1"/>
-    <col min="22" max="22" width="15.109375" customWidth="1"/>
-    <col min="23" max="23" width="21.33203125" customWidth="1"/>
-    <col min="24" max="24" width="23.5546875" customWidth="1"/>
-    <col min="25" max="25" width="19.109375" customWidth="1"/>
+    <col min="17" max="17" width="9.25" customWidth="1"/>
+    <col min="18" max="18" width="14.5" customWidth="1"/>
+    <col min="19" max="19" width="17.25" customWidth="1"/>
+    <col min="20" max="20" width="19.625" customWidth="1"/>
+    <col min="21" max="21" width="22.875" customWidth="1"/>
+    <col min="22" max="22" width="15.125" customWidth="1"/>
+    <col min="23" max="23" width="21.375" customWidth="1"/>
+    <col min="24" max="24" width="23.5" customWidth="1"/>
+    <col min="25" max="25" width="19.125" customWidth="1"/>
     <col min="26" max="26" width="22" customWidth="1"/>
-    <col min="27" max="29" width="22.88671875" customWidth="1"/>
-    <col min="30" max="30" width="24.77734375" customWidth="1"/>
-    <col min="31" max="31" width="25.88671875" customWidth="1"/>
-    <col min="32" max="32" width="17.21875" customWidth="1"/>
-    <col min="33" max="33" width="15.109375" customWidth="1"/>
-    <col min="34" max="34" width="16.5546875" customWidth="1"/>
-    <col min="35" max="35" width="12.33203125" customWidth="1"/>
+    <col min="27" max="29" width="22.875" customWidth="1"/>
+    <col min="30" max="30" width="24.75" customWidth="1"/>
+    <col min="31" max="31" width="25.875" customWidth="1"/>
+    <col min="32" max="32" width="17.25" customWidth="1"/>
+    <col min="33" max="33" width="15.125" customWidth="1"/>
+    <col min="34" max="34" width="16.5" customWidth="1"/>
+    <col min="35" max="35" width="12.375" customWidth="1"/>
     <col min="36" max="36" width="13" customWidth="1"/>
     <col min="37" max="37" width="15" customWidth="1"/>
-    <col min="38" max="38" width="30.21875" customWidth="1"/>
-    <col min="39" max="39" width="15.33203125" customWidth="1"/>
-    <col min="40" max="40" width="23.6640625" customWidth="1"/>
-    <col min="41" max="41" width="18.77734375" customWidth="1"/>
-    <col min="42" max="42" width="21.21875" customWidth="1"/>
-    <col min="43" max="43" width="22.109375" customWidth="1"/>
-    <col min="44" max="44" width="25.6640625" customWidth="1"/>
-    <col min="45" max="45" width="31.44140625" customWidth="1"/>
-    <col min="46" max="46" width="39.109375" customWidth="1"/>
-    <col min="47" max="47" width="16.109375" customWidth="1"/>
-    <col min="48" max="48" width="27.33203125" customWidth="1"/>
+    <col min="38" max="38" width="30.25" customWidth="1"/>
+    <col min="39" max="39" width="15.375" customWidth="1"/>
+    <col min="40" max="40" width="23.625" customWidth="1"/>
+    <col min="41" max="41" width="18.75" customWidth="1"/>
+    <col min="42" max="42" width="21.25" customWidth="1"/>
+    <col min="43" max="43" width="22.125" customWidth="1"/>
+    <col min="44" max="44" width="25.625" customWidth="1"/>
+    <col min="45" max="45" width="31.5" customWidth="1"/>
+    <col min="46" max="46" width="39.125" customWidth="1"/>
+    <col min="47" max="47" width="16.125" customWidth="1"/>
+    <col min="48" max="48" width="27.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:48" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="8"/>
-      <c r="AL1" s="8"/>
-      <c r="AM1" s="8"/>
-      <c r="AN1" s="8"/>
-      <c r="AO1" s="8"/>
-      <c r="AP1" s="8"/>
-      <c r="AQ1" s="8"/>
-      <c r="AR1" s="8"/>
-      <c r="AS1" s="8"/>
-      <c r="AT1" s="8"/>
-      <c r="AU1" s="8"/>
-      <c r="AV1" s="8"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5"/>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+      <c r="AU1" s="5"/>
+      <c r="AV1" s="5"/>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:48" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9"/>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="9"/>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="9"/>
-      <c r="AO2" s="9"/>
-      <c r="AP2" s="9"/>
-      <c r="AQ2" s="9"/>
-      <c r="AR2" s="9"/>
-      <c r="AS2" s="9"/>
-      <c r="AT2" s="9"/>
-      <c r="AU2" s="9"/>
-      <c r="AV2" s="9"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
+      <c r="AK2" s="6"/>
+      <c r="AL2" s="6"/>
+      <c r="AM2" s="6"/>
+      <c r="AN2" s="6"/>
+      <c r="AO2" s="6"/>
+      <c r="AP2" s="6"/>
+      <c r="AQ2" s="6"/>
+      <c r="AR2" s="6"/>
+      <c r="AS2" s="6"/>
+      <c r="AT2" s="6"/>
+      <c r="AU2" s="6"/>
+      <c r="AV2" s="6"/>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:48" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -788,201 +803,201 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="M4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="S4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="T4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="U4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="V4" s="4" t="s">
+      <c r="V4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="W4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="X4" s="4" t="s">
+      <c r="X4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Y4" s="4" t="s">
+      <c r="Y4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Z4" s="4" t="s">
+      <c r="Z4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AA4" s="4" t="s">
+      <c r="AA4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AB4" s="4" t="s">
+      <c r="AB4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AC4" s="4" t="s">
+      <c r="AC4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="AD4" s="4" t="s">
+      <c r="AD4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AE4" s="4" t="s">
+      <c r="AE4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AF4" s="4" t="s">
+      <c r="AF4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AG4" s="4" t="s">
+      <c r="AG4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="AH4" s="4" t="s">
+      <c r="AH4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AI4" s="4" t="s">
+      <c r="AI4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="AJ4" s="4" t="s">
+      <c r="AJ4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AK4" s="4" t="s">
+      <c r="AK4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AL4" s="4" t="s">
+      <c r="AL4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="AM4" s="4" t="s">
+      <c r="AM4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AN4" s="4" t="s">
+      <c r="AN4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AO4" s="4" t="s">
+      <c r="AO4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="AP4" s="4" t="s">
+      <c r="AP4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="AQ4" s="4" t="s">
+      <c r="AQ4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AR4" s="4" t="s">
+      <c r="AR4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AS4" s="4" t="s">
+      <c r="AS4" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AT4" s="4" t="s">
+      <c r="AT4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AU4" s="4" t="s">
+      <c r="AU4" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AV4" s="4" t="s">
+      <c r="AV4" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:48" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="5"/>
-      <c r="AG5" s="5"/>
-      <c r="AH5" s="5"/>
-      <c r="AI5" s="5"/>
-      <c r="AJ5" s="5"/>
-      <c r="AK5" s="5"/>
-      <c r="AL5" s="5"/>
-      <c r="AM5" s="5"/>
-      <c r="AN5" s="5"/>
-      <c r="AO5" s="5"/>
-      <c r="AP5" s="5"/>
-      <c r="AQ5" s="5"/>
-      <c r="AR5" s="5"/>
-      <c r="AS5" s="5"/>
-      <c r="AT5" s="5"/>
-      <c r="AU5" s="5"/>
-      <c r="AV5" s="5"/>
+    <row r="5" spans="1:48" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="8"/>
+      <c r="AE5" s="8"/>
+      <c r="AF5" s="8"/>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="8"/>
+      <c r="AJ5" s="8"/>
+      <c r="AK5" s="8"/>
+      <c r="AL5" s="8"/>
+      <c r="AM5" s="8"/>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="8"/>
+      <c r="AP5" s="8"/>
+      <c r="AQ5" s="8"/>
+      <c r="AR5" s="8"/>
+      <c r="AS5" s="8"/>
+      <c r="AT5" s="8"/>
+      <c r="AU5" s="8"/>
+      <c r="AV5" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
update bang ke chi tiet hoa don excel
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/HoaDonDienTu/BANG_KE_CHI_TIET_HOA_DON_DIEN_TU.xlsx
+++ b/API/wwwroot/docs/HoaDonDienTu/BANG_KE_CHI_TIET_HOA_DON_DIEN_TU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bill-back-end\API\wwwroot\docs\HoaDonDienTu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A91715-437E-41CA-9982-DC7004C153F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9880D4-7974-4449-9179-B6415F182281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -309,18 +309,14 @@
       <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,7 +635,7 @@
   <dimension ref="A1:AV5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -692,108 +688,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:48" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
-      <c r="AG1" s="5"/>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5"/>
-      <c r="AM1" s="5"/>
-      <c r="AN1" s="5"/>
-      <c r="AO1" s="5"/>
-      <c r="AP1" s="5"/>
-      <c r="AQ1" s="5"/>
-      <c r="AR1" s="5"/>
-      <c r="AS1" s="5"/>
-      <c r="AT1" s="5"/>
-      <c r="AU1" s="5"/>
-      <c r="AV1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="8"/>
+      <c r="AP1" s="8"/>
+      <c r="AQ1" s="8"/>
+      <c r="AR1" s="8"/>
+      <c r="AS1" s="8"/>
+      <c r="AT1" s="8"/>
+      <c r="AU1" s="8"/>
+      <c r="AV1" s="8"/>
     </row>
     <row r="2" spans="1:48" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6"/>
-      <c r="AH2" s="6"/>
-      <c r="AI2" s="6"/>
-      <c r="AJ2" s="6"/>
-      <c r="AK2" s="6"/>
-      <c r="AL2" s="6"/>
-      <c r="AM2" s="6"/>
-      <c r="AN2" s="6"/>
-      <c r="AO2" s="6"/>
-      <c r="AP2" s="6"/>
-      <c r="AQ2" s="6"/>
-      <c r="AR2" s="6"/>
-      <c r="AS2" s="6"/>
-      <c r="AT2" s="6"/>
-      <c r="AU2" s="6"/>
-      <c r="AV2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
+      <c r="AI2" s="7"/>
+      <c r="AJ2" s="7"/>
+      <c r="AK2" s="7"/>
+      <c r="AL2" s="7"/>
+      <c r="AM2" s="7"/>
+      <c r="AN2" s="7"/>
+      <c r="AO2" s="7"/>
+      <c r="AP2" s="7"/>
+      <c r="AQ2" s="7"/>
+      <c r="AR2" s="7"/>
+      <c r="AS2" s="7"/>
+      <c r="AT2" s="7"/>
+      <c r="AU2" s="7"/>
+      <c r="AV2" s="7"/>
     </row>
     <row r="3" spans="1:48" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
@@ -804,206 +800,202 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="O4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="P4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="Q4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="R4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="S4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="7" t="s">
+      <c r="T4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="7" t="s">
+      <c r="U4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="V4" s="7" t="s">
+      <c r="V4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="W4" s="7" t="s">
+      <c r="W4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="X4" s="7" t="s">
+      <c r="X4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Y4" s="7" t="s">
+      <c r="Y4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="Z4" s="7" t="s">
+      <c r="Z4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AA4" s="7" t="s">
+      <c r="AA4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AB4" s="7" t="s">
+      <c r="AB4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AC4" s="7" t="s">
+      <c r="AC4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AD4" s="7" t="s">
+      <c r="AD4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AE4" s="7" t="s">
+      <c r="AE4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AF4" s="7" t="s">
+      <c r="AF4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AG4" s="7" t="s">
+      <c r="AG4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AH4" s="7" t="s">
+      <c r="AH4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AI4" s="7" t="s">
+      <c r="AI4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AJ4" s="7" t="s">
+      <c r="AJ4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AK4" s="7" t="s">
+      <c r="AK4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AL4" s="7" t="s">
+      <c r="AL4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AM4" s="7" t="s">
+      <c r="AM4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AN4" s="7" t="s">
+      <c r="AN4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AO4" s="7" t="s">
+      <c r="AO4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AP4" s="7" t="s">
+      <c r="AP4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AQ4" s="7" t="s">
+      <c r="AQ4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AR4" s="7" t="s">
+      <c r="AR4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AS4" s="7" t="s">
+      <c r="AS4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AT4" s="7" t="s">
+      <c r="AT4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AU4" s="7" t="s">
+      <c r="AU4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AV4" s="7" t="s">
+      <c r="AV4" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:48" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
-      <c r="AC5" s="8"/>
-      <c r="AD5" s="8"/>
-      <c r="AE5" s="8"/>
-      <c r="AF5" s="8"/>
-      <c r="AG5" s="8"/>
-      <c r="AH5" s="8"/>
-      <c r="AI5" s="8"/>
-      <c r="AJ5" s="8"/>
-      <c r="AK5" s="8"/>
-      <c r="AL5" s="8"/>
-      <c r="AM5" s="8"/>
-      <c r="AN5" s="8"/>
-      <c r="AO5" s="8"/>
-      <c r="AP5" s="8"/>
-      <c r="AQ5" s="8"/>
-      <c r="AR5" s="8"/>
-      <c r="AS5" s="8"/>
-      <c r="AT5" s="8"/>
-      <c r="AU5" s="8"/>
-      <c r="AV5" s="8"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="6"/>
+      <c r="AL5" s="6"/>
+      <c r="AM5" s="6"/>
+      <c r="AN5" s="6"/>
+      <c r="AO5" s="6"/>
+      <c r="AP5" s="6"/>
+      <c r="AQ5" s="6"/>
+      <c r="AR5" s="6"/>
+      <c r="AS5" s="6"/>
+      <c r="AT5" s="6"/>
+      <c r="AU5" s="6"/>
+      <c r="AV5" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:AV1"/>
-    <mergeCell ref="A2:AV2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Bug #2395: 0.9.Khac phuc HDBK T08.2022 - LK 2022-08-02
</commit_message>
<xml_diff>
--- a/API/wwwroot/docs/HoaDonDienTu/BANG_KE_CHI_TIET_HOA_DON_DIEN_TU.xlsx
+++ b/API/wwwroot/docs/HoaDonDienTu/BANG_KE_CHI_TIET_HOA_DON_DIEN_TU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\bill-back-end\API\wwwroot\docs\HoaDonDienTu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9880D4-7974-4449-9179-B6415F182281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D545A2A-6842-4831-810D-10DBBE2D054B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>BẢNG KÊ CHI TIẾT HÓA ĐƠN ĐIỆN TỬ</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Trạng thái hóa đơn</t>
   </si>
   <si>
-    <t>Trạng thái phát hành</t>
-  </si>
-  <si>
     <t>Mã tra cứu</t>
   </si>
   <si>
@@ -183,6 +180,12 @@
   </si>
   <si>
     <t>Thông tin hóa đơn liên quan</t>
+  </si>
+  <si>
+    <t>Mã CQT cấp</t>
+  </si>
+  <si>
+    <t>Trạng thái quy trình</t>
   </si>
 </sst>
 </file>
@@ -632,10 +635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AV5"/>
+  <dimension ref="A1:AW5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -681,13 +684,14 @@
     <col min="42" max="42" width="21.25" customWidth="1"/>
     <col min="43" max="43" width="22.125" customWidth="1"/>
     <col min="44" max="44" width="25.625" customWidth="1"/>
-    <col min="45" max="45" width="31.5" customWidth="1"/>
-    <col min="46" max="46" width="39.125" customWidth="1"/>
-    <col min="47" max="47" width="16.125" customWidth="1"/>
-    <col min="48" max="48" width="27.375" customWidth="1"/>
+    <col min="45" max="45" width="37.875" customWidth="1"/>
+    <col min="46" max="46" width="31.5" customWidth="1"/>
+    <col min="47" max="47" width="39.125" customWidth="1"/>
+    <col min="48" max="48" width="16.125" customWidth="1"/>
+    <col min="49" max="49" width="27.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:49" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -738,8 +742,9 @@
       <c r="AT1" s="8"/>
       <c r="AU1" s="8"/>
       <c r="AV1" s="8"/>
+      <c r="AW1" s="8"/>
     </row>
-    <row r="2" spans="1:48" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -790,8 +795,9 @@
       <c r="AT2" s="7"/>
       <c r="AU2" s="7"/>
       <c r="AV2" s="7"/>
+      <c r="AW2" s="7"/>
     </row>
-    <row r="3" spans="1:48" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:49" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -799,7 +805,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -846,7 +852,7 @@
         <v>16</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q4" s="5" t="s">
         <v>17</v>
@@ -882,10 +888,10 @@
         <v>27</v>
       </c>
       <c r="AB4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC4" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="AC4" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="AD4" s="5" t="s">
         <v>28</v>
@@ -927,25 +933,28 @@
         <v>40</v>
       </c>
       <c r="AQ4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AR4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AR4" s="5" t="s">
+      <c r="AS4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AS4" s="5" t="s">
+      <c r="AU4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AV4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AT4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="AU4" s="5" t="s">
+      <c r="AW4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AV4" s="5" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="5" spans="1:48" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:49" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -994,6 +1003,7 @@
       <c r="AT5" s="6"/>
       <c r="AU5" s="6"/>
       <c r="AV5" s="6"/>
+      <c r="AW5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>